<commit_message>
XML-feat: thread models versions updated
</commit_message>
<xml_diff>
--- a/post-microservice.xlsx
+++ b/post-microservice.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65466FA-42E9-43CD-9D52-5F31441CD3F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E777E05-DAB2-442F-B2F1-15435D5A6F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -906,9 +906,6 @@
     3) Admins, who can manipulate all the data that is marked as inappropriate which includes deleting posts and removing them permanently from registered user or agent profiles. Admin can view posts from all users with all privacy settings
     4) Other Nistagram Services, that transfer files to and from the Post microservice.
 The system is implemented with 10 microservices. All users interact with the system over HTTPS, using a web UI. Other Nistagram Services for communication rely on the REST protocol.</t>
-  </si>
-  <si>
-    <t>The backend is built using  Golang v1.16.3 within the GoLand 2020.3.3 IDE</t>
   </si>
   <si>
     <t>1.8</t>
@@ -1195,6 +1192,9 @@
   </si>
   <si>
     <t>Updating post. POST request.</t>
+  </si>
+  <si>
+    <t>The backend is built using  Golang v1.15.3 within the GoLand 2021.1.1 IDE</t>
   </si>
 </sst>
 </file>
@@ -1883,9 +1883,30 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="18" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1916,27 +1937,6 @@
     <xf numFmtId="49" fontId="8" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1970,14 +1970,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1988,17 +1997,8 @@
     <xf numFmtId="49" fontId="7" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2718,8 +2718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O90"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2736,8 +2736,8 @@
       <c r="A1" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="84"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="85"/>
       <c r="D1" s="40"/>
     </row>
     <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2758,10 +2758,10 @@
       <c r="A3" s="13">
         <v>1</v>
       </c>
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="94"/>
+      <c r="C3" s="101"/>
       <c r="D3" s="63"/>
     </row>
     <row r="4" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -2811,7 +2811,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="59" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C7" s="52" t="s">
         <v>262</v>
@@ -2825,7 +2825,7 @@
         <v>259</v>
       </c>
       <c r="B8" s="59" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C8" s="62" t="s">
         <v>264</v>
@@ -2842,23 +2842,23 @@
         <v>260</v>
       </c>
       <c r="C9" s="59" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D9" s="61" t="s">
         <v>133</v>
       </c>
-      <c r="F9" s="85" t="s">
+      <c r="F9" s="92" t="s">
         <v>142</v>
       </c>
-      <c r="G9" s="86"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="86"/>
-      <c r="K9" s="86"/>
-      <c r="L9" s="86"/>
-      <c r="M9" s="86"/>
-      <c r="N9" s="86"/>
-      <c r="O9" s="87"/>
+      <c r="G9" s="93"/>
+      <c r="H9" s="93"/>
+      <c r="I9" s="93"/>
+      <c r="J9" s="93"/>
+      <c r="K9" s="93"/>
+      <c r="L9" s="93"/>
+      <c r="M9" s="93"/>
+      <c r="N9" s="93"/>
+      <c r="O9" s="94"/>
     </row>
     <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="60" t="s">
@@ -2868,31 +2868,31 @@
         <v>261</v>
       </c>
       <c r="C10" s="59" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D10" s="61">
         <v>1.3</v>
       </c>
-      <c r="F10" s="88"/>
-      <c r="G10" s="89"/>
-      <c r="H10" s="89"/>
-      <c r="I10" s="89"/>
-      <c r="J10" s="89"/>
-      <c r="K10" s="89"/>
-      <c r="L10" s="89"/>
-      <c r="M10" s="89"/>
-      <c r="N10" s="89"/>
-      <c r="O10" s="90"/>
+      <c r="F10" s="95"/>
+      <c r="G10" s="96"/>
+      <c r="H10" s="96"/>
+      <c r="I10" s="96"/>
+      <c r="J10" s="96"/>
+      <c r="K10" s="96"/>
+      <c r="L10" s="96"/>
+      <c r="M10" s="96"/>
+      <c r="N10" s="96"/>
+      <c r="O10" s="97"/>
     </row>
     <row r="11" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="60" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B11" s="59" t="s">
+        <v>299</v>
+      </c>
+      <c r="C11" s="59" t="s">
         <v>300</v>
-      </c>
-      <c r="C11" s="59" t="s">
-        <v>301</v>
       </c>
       <c r="D11" s="61" t="s">
         <v>134</v>
@@ -2902,10 +2902,10 @@
       <c r="A12" s="12">
         <v>2</v>
       </c>
-      <c r="B12" s="91" t="s">
+      <c r="B12" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="92"/>
+      <c r="C12" s="99"/>
       <c r="D12" s="63"/>
     </row>
     <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -2913,10 +2913,10 @@
         <v>16</v>
       </c>
       <c r="B13" s="59" t="s">
+        <v>301</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>302</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>303</v>
       </c>
       <c r="D13" s="61"/>
     </row>
@@ -2939,10 +2939,10 @@
         <v>20</v>
       </c>
       <c r="B15" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="C15" s="29" t="s">
         <v>304</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>305</v>
       </c>
       <c r="D15" s="61" t="s">
         <v>134</v>
@@ -2956,7 +2956,7 @@
         <v>54</v>
       </c>
       <c r="C16" s="50" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D16" s="61" t="s">
         <v>134</v>
@@ -2967,10 +2967,10 @@
         <v>59</v>
       </c>
       <c r="B17" s="59" t="s">
+        <v>307</v>
+      </c>
+      <c r="C17" s="59" t="s">
         <v>308</v>
-      </c>
-      <c r="C17" s="59" t="s">
-        <v>309</v>
       </c>
       <c r="D17" s="61" t="s">
         <v>133</v>
@@ -3007,7 +3007,7 @@
         <v>75</v>
       </c>
       <c r="B20" s="59" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C20" s="55" t="s">
         <v>76</v>
@@ -3018,10 +3018,10 @@
       <c r="A21" s="12">
         <v>3</v>
       </c>
-      <c r="B21" s="91" t="s">
+      <c r="B21" s="98" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="92"/>
+      <c r="C21" s="99"/>
       <c r="D21" s="63"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3083,10 +3083,10 @@
         <v>65</v>
       </c>
       <c r="B26" s="59" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C26" s="59" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D26" s="61">
         <v>4</v>
@@ -3097,7 +3097,7 @@
         <v>129</v>
       </c>
       <c r="B27" s="59" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C27" s="65" t="s">
         <v>255</v>
@@ -3111,19 +3111,19 @@
         <v>135</v>
       </c>
       <c r="B28" s="59" t="s">
+        <v>312</v>
+      </c>
+      <c r="C28" s="59" t="s">
         <v>313</v>
       </c>
-      <c r="C28" s="59" t="s">
-        <v>314</v>
-      </c>
       <c r="D28" s="61"/>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="96" t="s">
+      <c r="A29" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="96"/>
-      <c r="C29" s="96"/>
+      <c r="B29" s="86"/>
+      <c r="C29" s="86"/>
       <c r="D29" s="40"/>
     </row>
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3173,7 +3173,7 @@
         <v>70</v>
       </c>
       <c r="B33" s="59" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C33" s="50" t="s">
         <v>179</v>
@@ -3187,7 +3187,7 @@
         <v>71</v>
       </c>
       <c r="B34" s="59" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C34" s="50" t="s">
         <v>180</v>
@@ -3201,7 +3201,7 @@
         <v>72</v>
       </c>
       <c r="B35" s="59" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C35" s="50" t="s">
         <v>181</v>
@@ -3215,7 +3215,7 @@
         <v>73</v>
       </c>
       <c r="B36" s="59" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C36" s="50" t="s">
         <v>182</v>
@@ -3299,7 +3299,7 @@
         <v>223</v>
       </c>
       <c r="B42" s="59" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C42" s="50" t="s">
         <v>191</v>
@@ -3341,7 +3341,7 @@
         <v>226</v>
       </c>
       <c r="B45" s="59" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C45" s="50" t="s">
         <v>192</v>
@@ -3355,7 +3355,7 @@
         <v>227</v>
       </c>
       <c r="B46" s="59" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C46" s="50" t="s">
         <v>193</v>
@@ -3599,7 +3599,7 @@
         <v>207</v>
       </c>
       <c r="D63" s="61" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3613,7 +3613,7 @@
         <v>208</v>
       </c>
       <c r="D64" s="61" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -3627,7 +3627,7 @@
         <v>209</v>
       </c>
       <c r="D65" s="61" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -3641,7 +3641,7 @@
         <v>210</v>
       </c>
       <c r="D66" s="61" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3744,13 +3744,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="76" t="s">
+        <v>366</v>
+      </c>
+      <c r="B74" s="75" t="s">
+        <v>365</v>
+      </c>
+      <c r="C74" s="77" t="s">
         <v>367</v>
-      </c>
-      <c r="B74" s="75" t="s">
-        <v>366</v>
-      </c>
-      <c r="C74" s="77" t="s">
-        <v>368</v>
       </c>
       <c r="D74" s="61" t="s">
         <v>133</v>
@@ -3770,86 +3770,86 @@
       <c r="B76" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="C76" s="84"/>
+      <c r="C76" s="85"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="B77" s="99" t="s">
+      <c r="B77" s="89" t="s">
         <v>27</v>
       </c>
-      <c r="C77" s="99"/>
+      <c r="C77" s="89"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="B78" s="100" t="s">
+      <c r="B78" s="90" t="s">
         <v>79</v>
       </c>
-      <c r="C78" s="101"/>
+      <c r="C78" s="91"/>
     </row>
     <row r="79" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="B79" s="100" t="s">
+      <c r="B79" s="90" t="s">
         <v>77</v>
       </c>
-      <c r="C79" s="101"/>
+      <c r="C79" s="91"/>
     </row>
     <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="B80" s="99" t="s">
+      <c r="B80" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="C80" s="99"/>
+      <c r="C80" s="89"/>
     </row>
     <row r="81" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="B81" s="97" t="s">
-        <v>294</v>
-      </c>
-      <c r="C81" s="98"/>
+      <c r="B81" s="87" t="s">
+        <v>368</v>
+      </c>
+      <c r="C81" s="88"/>
     </row>
     <row r="82" spans="1:3" ht="154.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="B82" s="97" t="s">
-        <v>355</v>
-      </c>
-      <c r="C82" s="98"/>
+      <c r="B82" s="87" t="s">
+        <v>354</v>
+      </c>
+      <c r="C82" s="88"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="B83" s="98" t="s">
+      <c r="B83" s="88" t="s">
         <v>78</v>
       </c>
-      <c r="C83" s="98"/>
+      <c r="C83" s="88"/>
     </row>
     <row r="84" spans="1:3" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B84" s="97" t="s">
-        <v>350</v>
-      </c>
-      <c r="C84" s="98"/>
+      <c r="B84" s="87" t="s">
+        <v>349</v>
+      </c>
+      <c r="C84" s="88"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="44"/>
       <c r="B85" s="83" t="s">
         <v>291</v>
       </c>
-      <c r="C85" s="84"/>
+      <c r="C85" s="85"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="32" t="s">
@@ -3908,6 +3908,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="F9:O10"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B3:C3"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A29:C29"/>
     <mergeCell ref="B76:C76"/>
@@ -3919,11 +3924,6 @@
     <mergeCell ref="B79:C79"/>
     <mergeCell ref="B80:C80"/>
     <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="F9:O10"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4610,7 +4610,7 @@
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B45" s="111" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C45" s="111"/>
       <c r="D45" s="111"/>
@@ -5062,7 +5062,7 @@
     </row>
     <row r="75" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B75" s="111" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C75" s="111"/>
       <c r="D75" s="111"/>
@@ -5514,7 +5514,7 @@
     </row>
     <row r="105" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B105" s="111" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C105" s="111"/>
       <c r="D105" s="111"/>
@@ -5966,7 +5966,7 @@
     </row>
     <row r="135" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B135" s="111" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C135" s="111"/>
       <c r="D135" s="111"/>
@@ -6418,18 +6418,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B136:N164"/>
+    <mergeCell ref="B75:N75"/>
+    <mergeCell ref="B76:N104"/>
+    <mergeCell ref="B105:N105"/>
+    <mergeCell ref="B106:N134"/>
+    <mergeCell ref="B135:N135"/>
     <mergeCell ref="B46:N74"/>
     <mergeCell ref="B21:N21"/>
     <mergeCell ref="B2:N20"/>
     <mergeCell ref="B1:N1"/>
     <mergeCell ref="B22:N44"/>
     <mergeCell ref="B45:N45"/>
-    <mergeCell ref="B136:N164"/>
-    <mergeCell ref="B75:N75"/>
-    <mergeCell ref="B76:N104"/>
-    <mergeCell ref="B105:N105"/>
-    <mergeCell ref="B106:N134"/>
-    <mergeCell ref="B135:N135"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6454,12 +6454,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -6496,10 +6496,10 @@
       <c r="B4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="116" t="s">
+      <c r="C4" s="119" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="116"/>
+      <c r="D4" s="119"/>
     </row>
     <row r="5" spans="1:4" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -6508,10 +6508,10 @@
       <c r="B5" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="115" t="s">
+      <c r="C5" s="113" t="s">
         <v>98</v>
       </c>
-      <c r="D5" s="115"/>
+      <c r="D5" s="113"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -6548,10 +6548,10 @@
       <c r="B8" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="117" t="s">
+      <c r="C8" s="120" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="118"/>
+      <c r="D8" s="121"/>
     </row>
     <row r="9" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
@@ -6560,10 +6560,10 @@
       <c r="B9" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="C9" s="113" t="s">
+      <c r="C9" s="114" t="s">
         <v>87</v>
       </c>
-      <c r="D9" s="114"/>
+      <c r="D9" s="115"/>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
@@ -6572,34 +6572,34 @@
       <c r="B10" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="113" t="s">
+      <c r="C10" s="114" t="s">
         <v>138</v>
       </c>
-      <c r="D10" s="114"/>
+      <c r="D10" s="115"/>
     </row>
     <row r="11" spans="1:4" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>331</v>
-      </c>
-      <c r="C11" s="113" t="s">
         <v>330</v>
       </c>
-      <c r="D11" s="114"/>
+      <c r="C11" s="114" t="s">
+        <v>329</v>
+      </c>
+      <c r="D11" s="115"/>
     </row>
     <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="C12" s="114" t="s">
         <v>332</v>
       </c>
-      <c r="C12" s="113" t="s">
-        <v>333</v>
-      </c>
-      <c r="D12" s="114"/>
+      <c r="D12" s="115"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
@@ -6636,10 +6636,10 @@
       <c r="B15" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="119" t="s">
+      <c r="C15" s="116" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="119"/>
+      <c r="D15" s="116"/>
     </row>
     <row r="16" spans="1:4" ht="73.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
@@ -6648,10 +6648,10 @@
       <c r="B16" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="C16" s="115" t="s">
-        <v>334</v>
-      </c>
-      <c r="D16" s="115"/>
+      <c r="C16" s="113" t="s">
+        <v>333</v>
+      </c>
+      <c r="D16" s="113"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
@@ -6688,22 +6688,22 @@
       <c r="B19" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="119" t="s">
+      <c r="C19" s="116" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="119"/>
+      <c r="D19" s="116"/>
     </row>
     <row r="20" spans="1:4" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>102</v>
       </c>
       <c r="B20" s="56" t="s">
+        <v>334</v>
+      </c>
+      <c r="C20" s="113" t="s">
         <v>335</v>
       </c>
-      <c r="C20" s="115" t="s">
-        <v>336</v>
-      </c>
-      <c r="D20" s="115"/>
+      <c r="D20" s="113"/>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
@@ -6712,10 +6712,10 @@
       <c r="B21" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="113" t="s">
+      <c r="C21" s="114" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="114"/>
+      <c r="D21" s="115"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
@@ -6752,10 +6752,10 @@
       <c r="B24" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="119" t="s">
+      <c r="C24" s="116" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="120"/>
+      <c r="D24" s="122"/>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
@@ -6764,10 +6764,10 @@
       <c r="B25" s="47" t="s">
         <v>270</v>
       </c>
-      <c r="C25" s="113" t="s">
+      <c r="C25" s="114" t="s">
         <v>138</v>
       </c>
-      <c r="D25" s="114"/>
+      <c r="D25" s="115"/>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
@@ -6776,10 +6776,10 @@
       <c r="B26" s="49" t="s">
         <v>275</v>
       </c>
-      <c r="C26" s="113" t="s">
+      <c r="C26" s="114" t="s">
         <v>138</v>
       </c>
-      <c r="D26" s="114"/>
+      <c r="D26" s="115"/>
     </row>
     <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
@@ -6788,10 +6788,10 @@
       <c r="B27" s="49" t="s">
         <v>274</v>
       </c>
-      <c r="C27" s="113" t="s">
+      <c r="C27" s="114" t="s">
         <v>138</v>
       </c>
-      <c r="D27" s="114"/>
+      <c r="D27" s="115"/>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -6800,46 +6800,46 @@
       <c r="B28" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="C28" s="113" t="s">
+      <c r="C28" s="114" t="s">
         <v>266</v>
       </c>
-      <c r="D28" s="114"/>
+      <c r="D28" s="115"/>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B29" s="24" t="s">
         <v>282</v>
       </c>
-      <c r="C29" s="113" t="s">
+      <c r="C29" s="114" t="s">
         <v>285</v>
       </c>
-      <c r="D29" s="114"/>
+      <c r="D29" s="115"/>
     </row>
     <row r="30" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B30" s="24" t="s">
         <v>283</v>
       </c>
-      <c r="C30" s="113" t="s">
+      <c r="C30" s="114" t="s">
         <v>284</v>
       </c>
-      <c r="D30" s="114"/>
+      <c r="D30" s="115"/>
     </row>
     <row r="31" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B31" s="47" t="s">
         <v>271</v>
       </c>
-      <c r="C31" s="113" t="s">
+      <c r="C31" s="114" t="s">
         <v>138</v>
       </c>
-      <c r="D31" s="114"/>
+      <c r="D31" s="115"/>
     </row>
     <row r="32" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
@@ -6876,22 +6876,22 @@
       <c r="B34" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="119" t="s">
+      <c r="C34" s="116" t="s">
         <v>39</v>
       </c>
-      <c r="D34" s="120"/>
+      <c r="D34" s="122"/>
     </row>
     <row r="35" spans="1:4" ht="73.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
         <v>104</v>
       </c>
       <c r="B35" s="67" t="s">
-        <v>337</v>
-      </c>
-      <c r="C35" s="115" t="s">
+        <v>336</v>
+      </c>
+      <c r="C35" s="113" t="s">
         <v>118</v>
       </c>
-      <c r="D35" s="115"/>
+      <c r="D35" s="113"/>
     </row>
     <row r="36" spans="1:4" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="66" t="s">
@@ -6900,10 +6900,10 @@
       <c r="B36" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="113" t="s">
+      <c r="C36" s="114" t="s">
         <v>118</v>
       </c>
-      <c r="D36" s="114"/>
+      <c r="D36" s="115"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
@@ -6940,10 +6940,10 @@
       <c r="B39" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="119" t="s">
+      <c r="C39" s="116" t="s">
         <v>39</v>
       </c>
-      <c r="D39" s="119"/>
+      <c r="D39" s="116"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
@@ -6952,10 +6952,10 @@
       <c r="B40" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="C40" s="115" t="s">
+      <c r="C40" s="113" t="s">
         <v>89</v>
       </c>
-      <c r="D40" s="115"/>
+      <c r="D40" s="113"/>
     </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="s">
@@ -6964,22 +6964,22 @@
       <c r="B41" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="C41" s="115" t="s">
+      <c r="C41" s="113" t="s">
         <v>122</v>
       </c>
-      <c r="D41" s="115"/>
+      <c r="D41" s="113"/>
     </row>
     <row r="42" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="66" t="s">
+        <v>360</v>
+      </c>
+      <c r="B42" s="74" t="s">
+        <v>362</v>
+      </c>
+      <c r="C42" s="117" t="s">
         <v>361</v>
       </c>
-      <c r="B42" s="74" t="s">
-        <v>363</v>
-      </c>
-      <c r="C42" s="121" t="s">
-        <v>362</v>
-      </c>
-      <c r="D42" s="122"/>
+      <c r="D42" s="118"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
@@ -7016,10 +7016,10 @@
       <c r="B45" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C45" s="119" t="s">
+      <c r="C45" s="116" t="s">
         <v>39</v>
       </c>
-      <c r="D45" s="119"/>
+      <c r="D45" s="116"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
@@ -7028,10 +7028,10 @@
       <c r="B46" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="C46" s="115" t="s">
+      <c r="C46" s="113" t="s">
         <v>120</v>
       </c>
-      <c r="D46" s="115"/>
+      <c r="D46" s="113"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="25" t="s">
@@ -7068,10 +7068,10 @@
       <c r="B49" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C49" s="119" t="s">
+      <c r="C49" s="116" t="s">
         <v>39</v>
       </c>
-      <c r="D49" s="119"/>
+      <c r="D49" s="116"/>
     </row>
     <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="22" t="s">
@@ -7080,10 +7080,10 @@
       <c r="B50" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="C50" s="115" t="s">
-        <v>347</v>
-      </c>
-      <c r="D50" s="115"/>
+      <c r="C50" s="113" t="s">
+        <v>346</v>
+      </c>
+      <c r="D50" s="113"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="28" t="s">
@@ -7120,10 +7120,10 @@
       <c r="B53" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C53" s="119" t="s">
+      <c r="C53" s="116" t="s">
         <v>39</v>
       </c>
-      <c r="D53" s="119"/>
+      <c r="D53" s="116"/>
     </row>
     <row r="54" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="22" t="s">
@@ -7132,10 +7132,10 @@
       <c r="B54" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="C54" s="115" t="s">
+      <c r="C54" s="113" t="s">
         <v>93</v>
       </c>
-      <c r="D54" s="115"/>
+      <c r="D54" s="113"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="57" t="s">
@@ -7172,73 +7172,97 @@
       <c r="B57" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="C57" s="119" t="s">
+      <c r="C57" s="116" t="s">
         <v>39</v>
       </c>
-      <c r="D57" s="119"/>
+      <c r="D57" s="116"/>
     </row>
     <row r="58" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="22" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B58" s="56" t="s">
         <v>276</v>
       </c>
-      <c r="C58" s="115" t="s">
+      <c r="C58" s="113" t="s">
         <v>277</v>
       </c>
-      <c r="D58" s="115"/>
+      <c r="D58" s="113"/>
     </row>
     <row r="59" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="22" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B59" s="56" t="s">
         <v>267</v>
       </c>
-      <c r="C59" s="115" t="s">
+      <c r="C59" s="113" t="s">
         <v>268</v>
       </c>
-      <c r="D59" s="115"/>
+      <c r="D59" s="113"/>
     </row>
     <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="22" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B60" s="56" t="s">
         <v>278</v>
       </c>
-      <c r="C60" s="115" t="s">
+      <c r="C60" s="113" t="s">
         <v>279</v>
       </c>
-      <c r="D60" s="115"/>
+      <c r="D60" s="113"/>
     </row>
     <row r="61" spans="1:4" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="22" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B61" s="56" t="s">
         <v>280</v>
       </c>
-      <c r="C61" s="113" t="s">
+      <c r="C61" s="114" t="s">
         <v>281</v>
       </c>
-      <c r="D61" s="114"/>
+      <c r="D61" s="115"/>
     </row>
     <row r="62" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="66" t="s">
+        <v>357</v>
+      </c>
+      <c r="B62" s="72" t="s">
         <v>358</v>
       </c>
-      <c r="B62" s="72" t="s">
+      <c r="C62" s="114" t="s">
         <v>359</v>
       </c>
-      <c r="C62" s="113" t="s">
-        <v>360</v>
-      </c>
-      <c r="D62" s="114"/>
+      <c r="D62" s="115"/>
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C42:D42"/>
     <mergeCell ref="C59:D59"/>
     <mergeCell ref="C60:D60"/>
     <mergeCell ref="C28:D28"/>
@@ -7255,30 +7279,6 @@
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C61:D61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7289,7 +7289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -7302,15 +7302,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="86" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -7355,7 +7355,7 @@
         <v>116</v>
       </c>
       <c r="G3" s="69" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="116.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -7372,13 +7372,13 @@
         <v>41</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F4" s="53" t="s">
         <v>51</v>
       </c>
       <c r="G4" s="69" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7401,7 +7401,7 @@
         <v>116</v>
       </c>
       <c r="G5" s="69" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -7418,13 +7418,13 @@
         <v>41</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F6" s="69" t="s">
         <v>115</v>
       </c>
       <c r="G6" s="69" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="175.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7441,13 +7441,13 @@
         <v>41</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F7" s="26" t="s">
         <v>115</v>
       </c>
       <c r="G7" s="69" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7464,13 +7464,13 @@
         <v>50</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F8" s="26" t="s">
         <v>51</v>
       </c>
       <c r="G8" s="69" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7487,13 +7487,13 @@
         <v>37</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F9" s="26" t="s">
         <v>115</v>
       </c>
       <c r="G9" s="73" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7539,7 +7539,7 @@
         <v>116</v>
       </c>
       <c r="G11" s="69" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7579,13 +7579,13 @@
         <v>41</v>
       </c>
       <c r="E13" s="71" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F13" s="70" t="s">
         <v>115</v>
       </c>
       <c r="G13" s="70" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -7732,12 +7732,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7873,15 +7870,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34F3655E-FF67-4DBD-8937-399569529388}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BB517A3-CC67-477D-B6B3-FBDAE4AB9BBA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7905,10 +7906,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BB517A3-CC67-477D-B6B3-FBDAE4AB9BBA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34F3655E-FF67-4DBD-8937-399569529388}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>